<commit_message>
Zmieniono kryterium akceptacji TAP1.5
Pasek boczny ma się kurczyć, nie znikać
</commit_message>
<xml_diff>
--- a/Connector Testy Akceptacyjne.xlsx
+++ b/Connector Testy Akceptacyjne.xlsx
@@ -13,10 +13,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1756762367" val="1226" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1756762367" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1756762367" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1756762367"/>
+      <pm:revision xmlns:pm="smNativeData" day="1757844550" val="1228" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1757844550" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1757844550" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1757844550"/>
     </ext>
   </extLst>
 </workbook>
@@ -129,7 +129,55 @@
     <t>użytkownik kliknie przycisk zmiany widoczności menu bocznego raz, a po chwili ponownie</t>
   </si>
   <si>
-    <t>po pierwszym kliknięciu menu boczne przestanie być widoczne, a po drugim kliknięciu pojawia się w poprzednim miejscu i rozmiarze</t>
+    <r>
+      <t xml:space="preserve">po pierwszym kliknięciu menu boczne </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <charset val="0"/>
+        <family val="0"/>
+        <sz val="11"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </rPr>
+      <t>znacząco zmniejsza swoją szerokość (przynajmniej o połowę</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <charset val="0"/>
+        <family val="0"/>
+        <sz val="11"/>
+        <b val="0"/>
+        <i val="0"/>
+      </rPr>
+      <t xml:space="preserve">), a po drugim kliknięciu </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <charset val="0"/>
+        <family val="0"/>
+        <sz val="11"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </rPr>
+      <t>wraca do poprzedniego rozmiaru</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Aptos Narrow"/>
+        <charset val="0"/>
+        <family val="0"/>
+        <sz val="11"/>
+        <b val="0"/>
+        <i val="0"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
   <si>
     <t>TAP1.6</t>
@@ -206,15 +254,14 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1756762367" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1757844550" ulstyle="none" kern="1">
             <pm:latin face="Aptos Narrow" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -230,7 +277,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1756762367" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1757844550" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -240,16 +287,29 @@
     </font>
     <font>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <b/>
       <color rgb="FF000000"/>
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1756762367" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1757844550" ulstyle="none" kern="1">
             <pm:latin face="Aptos Narrow" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1757844550" fgClr="FF0000" ulstyle="none" kern="1">
+            <pm:latin face="Aptos Narrow" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -268,7 +328,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1756762367" type="1" fgLvl="100" fgClr="00D0D0D0" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1757844550" type="1" fgLvl="100" fgClr="00D0D0D0" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -291,7 +351,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1756762367" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1757844550" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -313,7 +373,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1756762367"/>
+          <pm:border xmlns:pm="smNativeData" id="1757844550"/>
         </ext>
       </extLst>
     </border>
@@ -332,7 +392,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1756762367"/>
+          <pm:border xmlns:pm="smNativeData" id="1757844550"/>
         </ext>
       </extLst>
     </border>
@@ -351,7 +411,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1756762367">
+          <pm:border xmlns:pm="smNativeData" id="1757844550">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -372,7 +432,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1756762367">
+          <pm:border xmlns:pm="smNativeData" id="1757844550">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -393,7 +453,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1756762367">
+          <pm:border xmlns:pm="smNativeData" id="1757844550">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -415,7 +475,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1756762367">
+          <pm:border xmlns:pm="smNativeData" id="1757844550">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -436,7 +496,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1756762367"/>
+          <pm:border xmlns:pm="smNativeData" id="1757844550"/>
         </ext>
       </extLst>
     </border>
@@ -444,18 +504,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -476,6 +530,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -483,10 +540,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1756762367" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1757844550" count="1">
         <pm:charStyle name="Normalny" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1756762367" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1757844550" count="1">
         <pm:color name="Kolor 24" rgb="D0D0D0"/>
       </pm:colors>
     </ext>
@@ -769,13 +826,13 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.60"/>
   <cols>
-    <col min="1" max="1" width="7.131148" customWidth="1" style="2"/>
-    <col min="2" max="2" width="41.057377" customWidth="1" style="2"/>
+    <col min="1" max="1" width="7.131148" customWidth="1" style="1"/>
+    <col min="2" max="2" width="41.057377" customWidth="1" style="1"/>
     <col min="3" max="3" width="23.360656" customWidth="1" style="1"/>
     <col min="4" max="4" width="19.549180" customWidth="1" style="1"/>
     <col min="5" max="5" width="38.483607" customWidth="1" style="1"/>
@@ -785,10 +842,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -797,7 +854,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -808,34 +865,34 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -846,29 +903,29 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -877,19 +934,19 @@
       <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -898,29 +955,29 @@
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -928,10 +985,10 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -940,7 +997,7 @@
       <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -951,10 +1008,10 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -963,7 +1020,7 @@
       <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -974,10 +1031,10 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -986,7 +1043,7 @@
       <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1000,7 +1057,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1756762367" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1757844550" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1009,10 +1066,10 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1756762367" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1756762367" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1756762367" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1756762367" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1757844550" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1757844550" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1757844550" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1757844550" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -1021,7 +1078,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1756762367" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1757844550" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>